<commit_message>
wip:pasos para crear formato resguardo
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/plantilla_resguardo.xlsx
+++ b/imagenes_guardadas/plantilla_resguardo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\acrivera-sis\imagenes_guardadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6211F81-3FCA-4AC8-846D-A07CD6FD295A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A5549-E685-41D7-9F25-46FDDBCB7E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6B656796-ED9C-4EED-AC0F-1AB662C7DB54}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>No. de Resguardo:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">061-00 LAPTOP </t>
   </si>
   <si>
     <t>Fecha de resguardo:</t>
@@ -106,9 +103,6 @@
 • Para el equipo de cómputo externo, el software permanecerá instalado mientras el empleado pertenezca a la empresa y el computador esté en sus manos, y en caso de renuncia o cambio de propietario sírvase presentar el equipo para la desinstalación del software propiedad de la empresa a fin de evitar responsabilidades posteriores. Para efectos de pérdida o robo del equipo mencionado deberá presentar acta del Ministerio Público correspondiente para anulación del presente resguardo.</t>
   </si>
   <si>
-    <t>auxiliar de soporte tecnico mayot</t>
-  </si>
-  <si>
     <t xml:space="preserve">José Arturo Moreno Aguilar </t>
   </si>
   <si>
@@ -121,18 +115,12 @@
     <t>Coordinador soporte</t>
   </si>
   <si>
-    <t>28-ENERO-20205</t>
-  </si>
-  <si>
     <t>Julio Castillo Valerdi</t>
   </si>
   <si>
     <t>Coordinador de sistemas</t>
   </si>
   <si>
-    <t>Jose Arturo Moreno aguilar mizadain hernandez</t>
-  </si>
-  <si>
     <t>Usuario.</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
   </si>
   <si>
     <t>ESTE RESGUARDO SUSTITUYE TODOS LOS ANTERIORES.</t>
-  </si>
-  <si>
-    <t>AS-FO-003</t>
   </si>
 </sst>
 </file>
@@ -484,7 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -505,9 +490,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,15 +508,123 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,110 +634,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,8 +722,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>115608</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>33131</xdr:rowOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>23606</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1099,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F484322-A350-4B33-975C-4B9DC04A139C}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="B9" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="B72" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1146,27 +1134,23 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="F7" s="6"/>
       <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="59" t="s">
-        <v>26</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="9" spans="1:13" ht="6" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="K9" s="7"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3"/>
@@ -1188,210 +1172,210 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2"/>
-      <c r="B11" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
+      <c r="B11" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
     </row>
     <row r="12" spans="1:13" ht="7.5" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
     </row>
     <row r="13" spans="1:13" ht="7.5" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
     </row>
     <row r="14" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
     </row>
     <row r="16" spans="1:13" ht="0.75" customHeight="1"/>
     <row r="17" spans="1:13" ht="18.75" customHeight="1">
-      <c r="B17" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
+      <c r="B17" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
     </row>
     <row r="18" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="19" spans="1:13" s="3" customFormat="1">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="F19" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="F19" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="21" spans="1:13" ht="15.2" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="22" t="s">
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="13" t="s">
+      <c r="L21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="M21" s="15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" ht="15.2" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:13" ht="15.2" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:13" ht="15.2" customHeight="1">
-      <c r="B25" s="13"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:13" ht="15.2" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="7.5" customHeight="1">
       <c r="B27" s="2"/>
@@ -1405,48 +1389,48 @@
     </row>
     <row r="28" spans="1:13" ht="3" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
       <c r="D28" s="2"/>
       <c r="E28" s="7"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="7.5" hidden="1" customHeight="1">
-      <c r="B29" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
+      <c r="B29" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
     </row>
     <row r="30" spans="1:13" ht="13.5" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
     </row>
     <row r="31" spans="1:13" ht="7.5" customHeight="1">
       <c r="B31" s="3"/>
@@ -1461,86 +1445,86 @@
     </row>
     <row r="32" spans="1:13" ht="14.45" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
+      <c r="B32" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
     </row>
     <row r="33" spans="1:13" ht="14.45" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="13" t="s">
+      <c r="L33" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L33" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="43"/>
+      <c r="M33" s="39"/>
     </row>
     <row r="34" spans="1:13" ht="14.45" customHeight="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="45"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
     </row>
     <row r="35" spans="1:13" ht="14.45" customHeight="1">
-      <c r="B35" s="17"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="45"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
     </row>
     <row r="36" spans="1:13" ht="14.45" customHeight="1">
-      <c r="B36" s="17"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="45"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="3.75" customHeight="1"/>
     <row r="38" spans="1:13" ht="13.5" hidden="1">
@@ -1554,385 +1538,395 @@
     </row>
     <row r="41" spans="1:13" ht="6" customHeight="1"/>
     <row r="42" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B42" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
+      <c r="B42" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
     </row>
     <row r="43" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
     </row>
     <row r="44" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
     </row>
     <row r="45" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
     </row>
     <row r="47" spans="1:13" ht="12" customHeight="1">
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
     </row>
     <row r="48" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
     </row>
     <row r="49" spans="1:13" ht="3.75" customHeight="1">
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
     </row>
     <row r="50" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
     </row>
     <row r="51" spans="1:13" ht="3.75" customHeight="1">
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
     </row>
     <row r="52" spans="1:13" ht="24" customHeight="1">
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="35"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
     </row>
     <row r="53" spans="1:13" ht="3.75" hidden="1" customHeight="1">
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
     </row>
     <row r="54" spans="1:13" ht="13.5" hidden="1" customHeight="1">
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
     </row>
     <row r="55" spans="1:13" ht="3.75" customHeight="1">
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B56" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="36" t="s">
+      <c r="B56" s="32"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="33"/>
+      <c r="H56" s="34"/>
+      <c r="J56" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G56" s="37"/>
-      <c r="H56" s="38"/>
-      <c r="J56" s="36" t="s">
+      <c r="K56" s="34"/>
+      <c r="L56" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K56" s="38"/>
-      <c r="L56" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M56" s="38"/>
+      <c r="M56" s="34"/>
     </row>
     <row r="57" spans="1:13" ht="12" customHeight="1">
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="41"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="41"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="41"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="37"/>
     </row>
     <row r="58" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B58" s="39" t="s">
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="39" t="s">
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
+      <c r="J58" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="40"/>
-      <c r="H58" s="41"/>
-      <c r="J58" s="39" t="s">
+      <c r="K58" s="37"/>
+      <c r="L58" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K58" s="41"/>
-      <c r="L58" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M58" s="41"/>
+      <c r="M58" s="37"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="41"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="41"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="41"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="37"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="B60" s="52"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="54"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="54"/>
-      <c r="H60" s="54"/>
-      <c r="I60" s="54"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="52"/>
-      <c r="M60" s="53"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="24"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="24"/>
     </row>
     <row r="61" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B61" s="52"/>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="53"/>
-      <c r="L61" s="52"/>
-      <c r="M61" s="53"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="24"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="24"/>
     </row>
     <row r="62" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B62" s="52"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="53"/>
-      <c r="L62" s="52"/>
-      <c r="M62" s="53"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="24"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="24"/>
     </row>
     <row r="63" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B63" s="52"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54"/>
-      <c r="J63" s="52"/>
-      <c r="K63" s="53"/>
-      <c r="L63" s="52"/>
-      <c r="M63" s="53"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="24"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="3"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="52"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="54"/>
-      <c r="J64" s="52"/>
-      <c r="K64" s="53"/>
-      <c r="L64" s="52"/>
-      <c r="M64" s="53"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="24"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="24"/>
     </row>
     <row r="65" spans="1:13" ht="34.5" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="53"/>
-      <c r="L65" s="52"/>
-      <c r="M65" s="53"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="24"/>
     </row>
     <row r="66" spans="1:13" ht="12.75" customHeight="1">
-      <c r="B66" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="G66" s="58"/>
-      <c r="H66" s="51"/>
-      <c r="J66" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="K66" s="51"/>
-      <c r="L66" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="M66" s="51"/>
+      <c r="B66" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="29"/>
+      <c r="H66" s="22"/>
+      <c r="J66" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="K66" s="22"/>
+      <c r="L66" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M66" s="22"/>
     </row>
     <row r="76" spans="1:13">
       <c r="B76" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
+        <v>30</v>
+      </c>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="80" spans="1:13" ht="0.75" customHeight="1"/>
+    <row r="81" hidden="1"/>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="L60:M65"/>
-    <mergeCell ref="B60:E65"/>
-    <mergeCell ref="F60:I65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="J60:K65"/>
-    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B11:M15"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B29:M30"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="B42:M54"/>
     <mergeCell ref="B56:E57"/>
     <mergeCell ref="B58:E59"/>
@@ -1949,28 +1943,14 @@
     <mergeCell ref="J58:K59"/>
     <mergeCell ref="L56:M57"/>
     <mergeCell ref="L58:M59"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B29:M30"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B11:M15"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="L60:M65"/>
+    <mergeCell ref="B60:E65"/>
+    <mergeCell ref="F60:I65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="J60:K65"/>
+    <mergeCell ref="J66:K66"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0" bottom="0" header="0" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
wip:creando las insercion de datos de resguardo
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/plantilla_resguardo.xlsx
+++ b/imagenes_guardadas/plantilla_resguardo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\acrivera-sis\imagenes_guardadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A5549-E685-41D7-9F25-46FDDBCB7E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7607A7-8FA1-4F7A-9BD6-4595A8609BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6B656796-ED9C-4EED-AC0F-1AB662C7DB54}"/>
   </bookViews>
@@ -469,7 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -514,8 +514,114 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,97 +650,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -665,8 +681,8 @@
       <xdr:rowOff>353668</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>248368</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1438993</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>57123</xdr:rowOff>
     </xdr:to>
@@ -1089,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F484322-A350-4B33-975C-4B9DC04A139C}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="B72" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L76" sqref="L76"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="B2" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1104,9 +1120,9 @@
     <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="1" customWidth="1"/>
     <col min="9" max="9" width="5" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="6" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="20" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="1" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1140,19 +1156,19 @@
       <c r="K7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="20"/>
+      <c r="L7" s="66"/>
     </row>
     <row r="8" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="9" spans="1:13" ht="6" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="21"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="7.5" hidden="1" customHeight="1">
@@ -1167,101 +1183,101 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2"/>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
     </row>
     <row r="12" spans="1:13" ht="7.5" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
     </row>
     <row r="13" spans="1:13" ht="7.5" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
     </row>
     <row r="14" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
     </row>
     <row r="16" spans="1:13" ht="0.75" customHeight="1"/>
     <row r="17" spans="1:13" ht="18.75" customHeight="1">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="19" spans="1:13" s="3" customFormat="1">
@@ -1269,11 +1285,12 @@
         <v>6</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="60"/>
+      <c r="G19" s="32"/>
       <c r="H19" s="13"/>
+      <c r="L19" s="22"/>
     </row>
     <row r="20" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="21" spans="1:13" ht="15.2" customHeight="1">
@@ -1281,100 +1298,100 @@
       <c r="B21" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="57" t="s">
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="59"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
       <c r="K21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="23" t="s">
         <v>12</v>
       </c>
       <c r="M21" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1">
+    <row r="22" spans="1:13" ht="26.25" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
+      <c r="L22" s="25"/>
       <c r="M22" s="19"/>
     </row>
-    <row r="23" spans="1:13" ht="15.2" customHeight="1">
+    <row r="23" spans="1:13" ht="26.25" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="19"/>
     </row>
-    <row r="24" spans="1:13" ht="15.2" customHeight="1">
+    <row r="24" spans="1:13" ht="26.25" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="18"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
+      <c r="L24" s="24"/>
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:13" ht="15.2" customHeight="1">
+    <row r="25" spans="1:13" ht="26.25" customHeight="1">
       <c r="B25" s="18"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
+      <c r="L25" s="24"/>
       <c r="M25" s="19"/>
     </row>
-    <row r="26" spans="1:13" ht="15.2" customHeight="1">
+    <row r="26" spans="1:13" ht="26.25" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
+      <c r="L26" s="24"/>
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="7.5" customHeight="1">
@@ -1385,52 +1402,52 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="L27" s="21"/>
     </row>
     <row r="28" spans="1:13" ht="3" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="2"/>
       <c r="E28" s="7"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="L28" s="21"/>
     </row>
     <row r="29" spans="1:13" ht="7.5" hidden="1" customHeight="1">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
     </row>
     <row r="30" spans="1:13" ht="13.5" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="1:13" ht="7.5" customHeight="1">
       <c r="B31" s="3"/>
@@ -1440,91 +1457,91 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="L31" s="22"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" ht="14.45" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
     </row>
     <row r="33" spans="1:13" ht="14.45" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
       <c r="K33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="L33" s="38" t="s">
+      <c r="L33" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="M33" s="39"/>
+      <c r="M33" s="50"/>
     </row>
     <row r="34" spans="1:13" ht="14.45" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="44"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="55"/>
       <c r="K34" s="17"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="41"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="52"/>
     </row>
     <row r="35" spans="1:13" ht="14.45" customHeight="1">
       <c r="B35" s="16"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="55"/>
       <c r="K35" s="17"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="41"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="52"/>
     </row>
     <row r="36" spans="1:13" ht="14.45" customHeight="1">
       <c r="B36" s="16"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="41"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="17"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="41"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="52"/>
     </row>
     <row r="37" spans="1:13" ht="3.75" customHeight="1"/>
     <row r="38" spans="1:13" ht="13.5" hidden="1">
@@ -1538,395 +1555,381 @@
     </row>
     <row r="41" spans="1:13" ht="6" customHeight="1"/>
     <row r="42" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
     </row>
     <row r="43" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
     </row>
     <row r="44" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="42"/>
+      <c r="M44" s="42"/>
     </row>
     <row r="45" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
     </row>
     <row r="47" spans="1:13" ht="12" customHeight="1">
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="42"/>
+      <c r="M47" s="42"/>
     </row>
     <row r="48" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="31"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="42"/>
+      <c r="M48" s="42"/>
     </row>
     <row r="49" spans="1:13" ht="3.75" customHeight="1">
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="31"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="31"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="42"/>
+      <c r="M49" s="42"/>
     </row>
     <row r="50" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
     </row>
     <row r="51" spans="1:13" ht="3.75" customHeight="1">
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="31"/>
-      <c r="L51" s="31"/>
-      <c r="M51" s="31"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="42"/>
+      <c r="M51" s="42"/>
     </row>
     <row r="52" spans="1:13" ht="24" customHeight="1">
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="31"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
     </row>
     <row r="53" spans="1:13" ht="3.75" hidden="1" customHeight="1">
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="31"/>
-      <c r="L53" s="31"/>
-      <c r="M53" s="31"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="42"/>
     </row>
     <row r="54" spans="1:13" ht="13.5" hidden="1" customHeight="1">
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="31"/>
-      <c r="M54" s="31"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
     </row>
     <row r="55" spans="1:13" ht="3.75" customHeight="1">
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B56" s="32"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="32" t="s">
+      <c r="B56" s="43"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="G56" s="33"/>
-      <c r="H56" s="34"/>
-      <c r="J56" s="32" t="s">
+      <c r="G56" s="44"/>
+      <c r="H56" s="45"/>
+      <c r="J56" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="K56" s="34"/>
-      <c r="L56" s="32" t="s">
+      <c r="K56" s="45"/>
+      <c r="L56" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="M56" s="34"/>
+      <c r="M56" s="45"/>
     </row>
     <row r="57" spans="1:13" ht="12" customHeight="1">
-      <c r="B57" s="35"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="37"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="37"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="48"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="48"/>
     </row>
     <row r="58" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B58" s="35"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="35" t="s">
+      <c r="B58" s="46"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="36"/>
-      <c r="H58" s="37"/>
-      <c r="J58" s="35" t="s">
+      <c r="G58" s="47"/>
+      <c r="H58" s="48"/>
+      <c r="J58" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K58" s="37"/>
-      <c r="L58" s="35" t="s">
+      <c r="K58" s="48"/>
+      <c r="L58" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="M58" s="37"/>
+      <c r="M58" s="48"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B59" s="35"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="37"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="37"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="48"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="48"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="B60" s="23"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="25"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="24"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="60"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="61"/>
+      <c r="I60" s="61"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="60"/>
     </row>
     <row r="61" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B61" s="23"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="25"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="24"/>
-      <c r="L61" s="23"/>
-      <c r="M61" s="24"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="60"/>
+      <c r="L61" s="59"/>
+      <c r="M61" s="60"/>
     </row>
     <row r="62" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B62" s="23"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="24"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="60"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="59"/>
+      <c r="M62" s="60"/>
     </row>
     <row r="63" spans="1:13" ht="7.5" customHeight="1">
-      <c r="B63" s="23"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="24"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="24"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="61"/>
+      <c r="H63" s="61"/>
+      <c r="I63" s="61"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="60"/>
+      <c r="L63" s="59"/>
+      <c r="M63" s="60"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="3"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="24"/>
+      <c r="B64" s="59"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="59"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="59"/>
+      <c r="K64" s="60"/>
+      <c r="L64" s="59"/>
+      <c r="M64" s="60"/>
     </row>
     <row r="65" spans="1:13" ht="34.5" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="25"/>
-      <c r="J65" s="23"/>
-      <c r="K65" s="24"/>
-      <c r="L65" s="23"/>
-      <c r="M65" s="24"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="61"/>
+      <c r="H65" s="61"/>
+      <c r="I65" s="61"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="60"/>
+      <c r="L65" s="59"/>
+      <c r="M65" s="60"/>
     </row>
     <row r="66" spans="1:13" ht="12.75" customHeight="1">
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="21" t="s">
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="G66" s="29"/>
-      <c r="H66" s="22"/>
-      <c r="J66" s="29" t="s">
+      <c r="G66" s="65"/>
+      <c r="H66" s="58"/>
+      <c r="J66" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="K66" s="22"/>
-      <c r="L66" s="21" t="s">
+      <c r="K66" s="58"/>
+      <c r="L66" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="M66" s="22"/>
+      <c r="M66" s="58"/>
     </row>
     <row r="76" spans="1:13">
       <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L76" s="2"/>
+      <c r="L76" s="21"/>
     </row>
     <row r="80" spans="1:13" ht="0.75" customHeight="1"/>
     <row r="81" hidden="1"/>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B11:M15"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B29:M30"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="L60:M65"/>
+    <mergeCell ref="B60:E65"/>
+    <mergeCell ref="F60:I65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="J60:K65"/>
+    <mergeCell ref="J66:K66"/>
     <mergeCell ref="B42:M54"/>
     <mergeCell ref="B56:E57"/>
     <mergeCell ref="B58:E59"/>
@@ -1943,14 +1946,28 @@
     <mergeCell ref="J58:K59"/>
     <mergeCell ref="L56:M57"/>
     <mergeCell ref="L58:M59"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="L60:M65"/>
-    <mergeCell ref="B60:E65"/>
-    <mergeCell ref="F60:I65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="J60:K65"/>
-    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B29:M30"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B11:M15"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0" bottom="0" header="0" footer="0.19685039370078741"/>

</xml_diff>